<commit_message>
Refreshing content for 2019 revisions
</commit_message>
<xml_diff>
--- a/2018_collar_data/COTS_Collars/collar_retrieval_notes.xlsx
+++ b/2018_collar_data/COTS_Collars/collar_retrieval_notes.xlsx
@@ -1,31 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason Karl\Documents\GitHub\COTS_GPS_Collars\collar_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jakal\OneDrive - University of Idaho\Documents\GitHub\COTS_GPS_Collars\COTS_GPS_Collars\2018_collar_data\COTS_Collars\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{924A958A-157A-44FC-BC37-F5374F540F75}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="8_{924A958A-157A-44FC-BC37-F5374F540F75}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{A1B5246F-E1C2-47E5-8F04-D7166BB948DE}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15473" windowHeight="6928" xr2:uid="{37DEF5DE-E62B-4F69-A89D-A21B679EA6DA}"/>
+    <workbookView xWindow="348" yWindow="348" windowWidth="17196" windowHeight="11916" xr2:uid="{37DEF5DE-E62B-4F69-A89D-A21B679EA6DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>Collar ID</t>
   </si>
@@ -82,6 +88,12 @@
   </si>
   <si>
     <t>iGotU collar notes</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Install date</t>
   </si>
 </sst>
 </file>
@@ -117,9 +129,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,23 +450,32 @@
   <dimension ref="A1:H26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="G2" sqref="G2:G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
         <v>8</v>
       </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -463,32 +485,72 @@
       <c r="D2" s="1">
         <v>43236</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E2" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F2">
+        <f>D2-E2</f>
+        <v>19</v>
+      </c>
+      <c r="G2">
+        <f>F2</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="D3" s="1">
         <v>43237</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F26" si="0">D3-E3</f>
+        <v>20</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G26" si="1">F3</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="D4" s="1">
         <v>43229</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E4" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="D5" s="1">
         <v>43224</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E5" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -501,8 +563,15 @@
       <c r="D6" s="1">
         <v>43218</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E6" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -512,8 +581,19 @@
       <c r="D7" s="1">
         <v>43235</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E7" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -523,8 +603,15 @@
       <c r="D8" s="1">
         <v>43224</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E8" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -534,8 +621,19 @@
       <c r="D9" s="1">
         <v>43227</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E9" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -545,8 +643,15 @@
       <c r="D10" s="1">
         <v>43225</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E10" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -556,8 +661,19 @@
       <c r="D11" s="1">
         <v>43232</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E11" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -567,16 +683,38 @@
       <c r="D12" s="1">
         <v>43231</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E12" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="D13" s="1">
         <v>43234</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E13" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -586,8 +724,19 @@
       <c r="D14" s="1">
         <v>43234</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E14" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -597,8 +746,19 @@
       <c r="D15" s="1">
         <v>43236</v>
       </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E15" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -608,8 +768,14 @@
       <c r="D16" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E16" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -622,8 +788,15 @@
       <c r="D17" s="1">
         <v>43225</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E17" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -636,16 +809,38 @@
       <c r="D18" s="1">
         <v>43240</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E18" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
       <c r="D19" s="1">
         <v>43236</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E19" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -655,8 +850,19 @@
       <c r="D20" s="1">
         <v>43232</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E20" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -669,16 +875,34 @@
       <c r="D21" s="1">
         <v>43230</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E21" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
       <c r="D22" s="1">
         <v>43232</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E22" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -691,19 +915,37 @@
       <c r="D23" s="1">
         <v>43226</v>
       </c>
+      <c r="E23" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
       <c r="H23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
       <c r="D24" s="1">
         <v>43229</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E24" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -713,8 +955,19 @@
       <c r="D25" s="1">
         <v>43231</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E25" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -723,6 +976,13 @@
       </c>
       <c r="D26" s="1">
         <v>43227</v>
+      </c>
+      <c r="E26" s="2">
+        <v>43217</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="0"/>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>